<commit_message>
Autocomplete para veículo e inclusão de novos ícones para mapa.
</commit_message>
<xml_diff>
--- a/itinerario/doc/Modelo.xlsx
+++ b/itinerario/doc/Modelo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="modelo" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Linha</t>
   </si>
@@ -127,6 +127,33 @@
   </si>
   <si>
     <t>diferença</t>
+  </si>
+  <si>
+    <t>rota</t>
+  </si>
+  <si>
+    <t>rota 001</t>
+  </si>
+  <si>
+    <t>hora ini</t>
+  </si>
+  <si>
+    <t>hora fim</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>calendário</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>ano letivo</t>
   </si>
 </sst>
 </file>
@@ -466,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -780,12 +807,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3">
+        <v>41397</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>